<commit_message>
update: single vintage year
</commit_message>
<xml_diff>
--- a/remix_nz/input/brownfield/power-plant-nz-database.xlsx
+++ b/remix_nz/input/brownfield/power-plant-nz-database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local\REMix\remix_nz\input\brownfield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7148F1EC-AE5A-4851-9574-7E1D41C45D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4B5810-1469-4611-834E-E43C85CB2695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1"/>
+    <workbookView minimized="1" xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15570" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="decom" sheetId="4" r:id="rId1"/>
@@ -19,10 +19,23 @@
     <sheet name="avg_gen" sheetId="5" r:id="rId4"/>
     <sheet name="power-plant-nz-database" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="30" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2575,10 +2588,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -3109,9 +3122,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3127,9 +3139,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -3197,7 +3209,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Rafaella Canessa Figueroa" refreshedDate="45307.473622337966" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="228">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Rafaella Canessa Figueroa" refreshedDate="45307.473622337966" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="228" xr:uid="{00000000-000A-0000-FFFF-FFFF1E000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -12566,7 +12578,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:J16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="38">
     <pivotField showAll="0"/>
@@ -12814,7 +12826,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="38">
     <pivotField showAll="0"/>
@@ -12946,7 +12958,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:J16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="38">
     <pivotField showAll="0"/>
@@ -13104,7 +13116,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:K16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="38">
     <pivotField showAll="0"/>
@@ -13368,52 +13380,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AL229" totalsRowShown="0">
-  <autoFilter ref="A1:AL229"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AL229" totalsRowShown="0">
+  <autoFilter ref="A1:AL229" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Wind"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A32:AJ48">
     <sortCondition ref="AI1:AI229"/>
   </sortState>
   <tableColumns count="38">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Type"/>
-    <tableColumn id="3" name="Primary_fuel"/>
-    <tableColumn id="4" name="Secondary_fuel"/>
-    <tableColumn id="5" name="Prime_mover_1"/>
-    <tableColumn id="6" name="Prime_mover_2"/>
-    <tableColumn id="7" name="Cogeneration"/>
-    <tableColumn id="8" name="Capacity_MW"/>
-    <tableColumn id="9" name="Largest_unit_MW"/>
-    <tableColumn id="10" name="Primary_efficiency"/>
-    <tableColumn id="11" name="Generating_units_number"/>
-    <tableColumn id="12" name="Generating_units_notes"/>
-    <tableColumn id="13" name="Year_built"/>
-    <tableColumn id="14" name="Status"/>
-    <tableColumn id="15" name="Cooling_type"/>
-    <tableColumn id="16" name="Cooling_source"/>
-    <tableColumn id="17" name="Group_name"/>
-    <tableColumn id="18" name="Group_order"/>
-    <tableColumn id="19" name="Owner_1"/>
-    <tableColumn id="20" name="Owner_2"/>
-    <tableColumn id="21" name="Operator"/>
-    <tableColumn id="22" name="Connection_type"/>
-    <tableColumn id="23" name="Avg_Ann_Gen_GWh"/>
-    <tableColumn id="24" name="Hydro_max_storage_m3"/>
-    <tableColumn id="25" name="Basin"/>
-    <tableColumn id="26" name="Regional_auth"/>
-    <tableColumn id="27" name="Region_name"/>
-    <tableColumn id="28" name="Island_name"/>
-    <tableColumn id="29" name="Node_name"/>
-    <tableColumn id="30" name="GIP substation"/>
-    <tableColumn id="31" name="Lifetime"/>
-    <tableColumn id="32" name="Lifetime_notes"/>
-    <tableColumn id="33" name="lat"/>
-    <tableColumn id="34" name="long"/>
-    <tableColumn id="35" name="Node"/>
-    <tableColumn id="36" name="Techs"/>
-    <tableColumn id="37" name="new_life" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Primary_fuel"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Secondary_fuel"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Prime_mover_1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Prime_mover_2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Cogeneration"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Capacity_MW"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Largest_unit_MW"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Primary_efficiency"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Generating_units_number"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Generating_units_notes"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Year_built"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Status"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cooling_type"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Cooling_source"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Group_name"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Group_order"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Owner_1"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Owner_2"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Operator"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Connection_type"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Avg_Ann_Gen_GWh"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Hydro_max_storage_m3"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Basin"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Regional_auth"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Region_name"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Island_name"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Node_name"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="GIP substation"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Lifetime"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Lifetime_notes"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="lat"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="long"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Node"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Techs"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="new_life" dataDxfId="1">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Lifetime]]&gt;2019,Table1[[#This Row],[Lifetime]],IF(Table1[[#This Row],[Year_built]]&gt;1,Table1[[#This Row],[Year_built]]+30,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" name="new_tech" dataDxfId="0">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="new_tech" dataDxfId="0">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Type]]="Hydroelectric","Hydro",Table1[[#This Row],[Techs]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13717,62 +13735,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD19"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="O5" sqref="O5:O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="10.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>805</v>
       </c>
       <c r="B1" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="W2" s="6" t="s">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="W2" s="5" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="W3" s="6" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>778</v>
       </c>
       <c r="B4" t="s">
@@ -13845,23 +13863,17 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>112</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1">
+      <c r="J5">
         <v>119</v>
       </c>
       <c r="K5" t="s">
@@ -13895,9 +13907,6 @@
         <f>CONCATENATE($K$5, ".loc[idx[","""",A5,"""",", [2020], ", """",$R$4,"""",, "], ", """", "unitsUpperLimit", """", "] = ",,IF(H5&gt;0,_xlfn.CONCAT(H5/1000, " # GW_el"),"0"))</f>
         <v>the_cap.loc[idx["AKL", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
       <c r="W5" t="s">
         <v>796</v>
       </c>
@@ -13930,25 +13939,20 @@
         <v>gt_cap.loc[idx["AKL", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>167</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1">
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6">
         <v>246.95</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6">
         <v>423.95</v>
       </c>
       <c r="K6" t="s">
@@ -13982,9 +13986,6 @@
         <f t="shared" ref="R6:R15" si="6">CONCATENATE($K$5, ".loc[idx[","""",A6,"""",", [2020], ", """",$R$4,"""",, "], ", """", "unitsUpperLimit", """", "] = ",,IF(H6&gt;0,_xlfn.CONCAT(H6/1000, " # GW_el"),"0"))</f>
         <v>the_cap.loc[idx["BOP", [2020], "OCGT"], "unitsUpperLimit"] = 0.01 # GW_el</v>
       </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
       <c r="W6" t="s">
         <v>795</v>
       </c>
@@ -14017,23 +14018,17 @@
         <v>gt_cap.loc[idx["BOP", [2020], "OCGT"], "unitsUpperLimit"] = 10 # GW_el</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>3.2</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1">
+      <c r="I7">
         <v>1728.9</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7">
         <v>1732.1000000000001</v>
       </c>
       <c r="L7" t="str">
@@ -14064,9 +14059,6 @@
         <f t="shared" si="6"/>
         <v>the_cap.loc[idx["CAN", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
       <c r="X7" t="str">
         <f t="shared" si="7"/>
         <v>gt_cap.loc[idx["CAN", [2020], "BIO"], "unitsUpperLimit"] = 3.2 # GW_el</v>
@@ -14096,21 +14088,14 @@
         <v>gt_cap.loc[idx["CAN", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1">
+      <c r="I8">
         <v>827.65</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8">
         <v>827.65</v>
       </c>
       <c r="L8" t="str">
@@ -14141,9 +14126,6 @@
         <f t="shared" si="6"/>
         <v>the_cap.loc[idx["CEN", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
       <c r="X8" t="str">
         <f t="shared" si="7"/>
         <v>gt_cap.loc[idx["CEN", [2020], "BIO"], "unitsUpperLimit"] = 0</v>
@@ -14173,23 +14155,17 @@
         <v>gt_cap.loc[idx["CEN", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>155</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1">
+      <c r="I9">
         <v>144.19999999999999</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9">
         <v>299.2</v>
       </c>
       <c r="L9" t="str">
@@ -14220,9 +14196,6 @@
         <f t="shared" si="6"/>
         <v>the_cap.loc[idx["HBY", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
       <c r="X9" t="str">
         <f t="shared" si="7"/>
         <v>gt_cap.loc[idx["HBY", [2020], "BIO"], "unitsUpperLimit"] = 0</v>
@@ -14252,21 +14225,14 @@
         <v>gt_cap.loc[idx["HBY", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1">
+      <c r="I10">
         <v>36.709999999999994</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10">
         <v>36.709999999999994</v>
       </c>
       <c r="L10" t="str">
@@ -14297,9 +14263,6 @@
         <f t="shared" si="6"/>
         <v>the_cap.loc[idx["NEL", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
       <c r="X10" t="str">
         <f t="shared" si="7"/>
         <v>gt_cap.loc[idx["NEL", [2020], "BIO"], "unitsUpperLimit"] = 0</v>
@@ -14329,23 +14292,17 @@
         <v>gt_cap.loc[idx["NEL", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>18</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>25</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1">
+      <c r="J11">
         <v>43</v>
       </c>
       <c r="L11" t="str">
@@ -14376,9 +14333,6 @@
         <f t="shared" si="6"/>
         <v>the_cap.loc[idx["NIS", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
       <c r="X11" t="str">
         <f t="shared" si="7"/>
         <v>gt_cap.loc[idx["NIS", [2020], "BIO"], "unitsUpperLimit"] = 0</v>
@@ -14408,21 +14362,14 @@
         <v>gt_cap.loc[idx["NIS", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1">
+      <c r="I12">
         <v>1813.9</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12">
         <v>1813.9</v>
       </c>
       <c r="L12" t="str">
@@ -14453,9 +14400,6 @@
         <f t="shared" si="6"/>
         <v>the_cap.loc[idx["OTG", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
       <c r="X12" t="str">
         <f t="shared" si="7"/>
         <v>gt_cap.loc[idx["OTG", [2020], "BIO"], "unitsUpperLimit"] = 0</v>
@@ -14485,27 +14429,23 @@
         <v>gt_cap.loc[idx["OTG", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>377</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1">
+      <c r="G13">
         <v>78.599999999999994</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13">
         <v>435</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13">
         <v>165.3</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13">
         <v>1055.9000000000001</v>
       </c>
       <c r="L13" t="str">
@@ -14536,9 +14476,6 @@
         <f t="shared" si="6"/>
         <v>the_cap.loc[idx["TRN", [2020], "OCGT"], "unitsUpperLimit"] = 0.435 # GW_el</v>
       </c>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
       <c r="X13" t="str">
         <f t="shared" si="7"/>
         <v>gt_cap.loc[idx["TRN", [2020], "BIO"], "unitsUpperLimit"] = 0</v>
@@ -14568,21 +14505,14 @@
         <v>gt_cap.loc[idx["TRN", [2020], "OCGT"], "unitsUpperLimit"] = 435 # GW_el</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1">
+      <c r="I14">
         <v>222.75</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14">
         <v>222.75</v>
       </c>
       <c r="L14" t="str">
@@ -14613,9 +14543,6 @@
         <f t="shared" si="6"/>
         <v>the_cap.loc[idx["WEL", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
       <c r="X14" t="str">
         <f t="shared" si="7"/>
         <v>gt_cap.loc[idx["WEL", [2020], "BIO"], "unitsUpperLimit"] = 0</v>
@@ -14645,31 +14572,29 @@
         <v>gt_cap.loc[idx["WEL", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>45.9</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>385</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>673</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15">
         <v>750</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15">
         <v>92</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15">
         <v>1072.7</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15">
         <v>3018.6000000000004</v>
       </c>
       <c r="L15" t="str">
@@ -14700,9 +14625,6 @@
         <f t="shared" si="6"/>
         <v>the_cap.loc[idx["WTO", [2020], "OCGT"], "unitsUpperLimit"] = 0.092 # GW_el</v>
       </c>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
       <c r="X15" t="str">
         <f>CONCATENATE($W$5, ".loc[idx[","""",A15,"""",", [2020], ", """",$X$4,"""",, "], ", """", "unitsUpperLimit", """", "] = ",IF(B15&gt;0,_xlfn.CONCAT(B15, " # GW_el"),"0"))</f>
         <v>gt_cap.loc[idx["WTO", [2020], "BIO"], "unitsUpperLimit"] = 45.9 # GW_el</v>
@@ -14732,42 +14654,39 @@
         <v>gt_cap.loc[idx["WTO", [2020], "OCGT"], "unitsUpperLimit"] = 92 # GW_el</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>56.099999999999994</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>762</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>112</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
         <v>173</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
         <v>865</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16">
         <v>828.6</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16">
         <v>537</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16">
         <v>6259.0599999999995</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16">
         <v>9592.76</v>
       </c>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
     </row>
-    <row r="17" spans="6:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>1036</v>
       </c>
@@ -14776,7 +14695,7 @@
         <v>gt_cap.loc[idx["", [2020], ""], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="19" spans="6:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:24" x14ac:dyDescent="0.25">
       <c r="X19" t="str">
         <f>X6</f>
         <v>gt_cap.loc[idx["BOP", [2020], "BIO"], "unitsUpperLimit"] = 0</v>
@@ -14788,35 +14707,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.36328125" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>778</v>
       </c>
       <c r="B3" t="s">
@@ -14833,19 +14752,19 @@
         <v>39725.599999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>134.49999999999997</v>
       </c>
-      <c r="C4" s="3" t="str">
+      <c r="C4" s="2" t="str">
         <f>A4</f>
         <v>AKL</v>
       </c>
       <c r="D4">
-        <f>B4/1000</f>
+        <f t="shared" ref="D4:D14" si="0">B4/1000</f>
         <v>0.13449999999999998</v>
       </c>
       <c r="F4" t="s">
@@ -14870,19 +14789,19 @@
         <v>807</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>506.25000000000006</v>
       </c>
-      <c r="C5" s="3" t="str">
-        <f t="shared" ref="C5:C14" si="0">A5</f>
+      <c r="C5" s="2" t="str">
+        <f t="shared" ref="C5:C14" si="1">A5</f>
         <v>BOP</v>
       </c>
       <c r="D5">
-        <f>B5/1000</f>
+        <f t="shared" si="0"/>
         <v>0.50625000000000009</v>
       </c>
       <c r="F5" t="s">
@@ -14897,24 +14816,24 @@
       <c r="K5">
         <v>5.3355800000000002</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="7">
         <f>K5/$L$14</f>
         <v>0.53880760247087356</v>
       </c>
       <c r="N5" t="s">
         <v>186</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="9">
         <v>9075.36</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="8">
         <f>O5/-$O$16</f>
         <v>0.22845117506091792</v>
       </c>
       <c r="Q5">
         <v>7835</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5" s="7">
         <v>0.1850714538797685</v>
       </c>
       <c r="T5" t="s">
@@ -14927,19 +14846,19 @@
         <v>9.8618164639187426E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>1757.7299999999998</v>
       </c>
-      <c r="C6" s="3" t="str">
+      <c r="C6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>CAN</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>CAN</v>
-      </c>
-      <c r="D6">
-        <f>B6/1000</f>
         <v>1.7577299999999998</v>
       </c>
       <c r="F6" t="s">
@@ -14954,24 +14873,24 @@
       <c r="K6">
         <v>1.06229</v>
       </c>
-      <c r="L6" s="8">
-        <f t="shared" ref="L6:L13" si="1">K6/$L$14</f>
+      <c r="L6" s="7">
+        <f t="shared" ref="L6:L13" si="2">K6/$L$14</f>
         <v>0.10727417226033238</v>
       </c>
       <c r="N6" t="s">
         <v>785</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9">
         <v>7515.01</v>
       </c>
-      <c r="P6" s="9">
-        <f t="shared" ref="P6:P13" si="2">O6/-$O$16</f>
+      <c r="P6" s="8">
+        <f t="shared" ref="P6:P13" si="3">O6/-$O$16</f>
         <v>0.18917297661961055</v>
       </c>
       <c r="Q6">
         <v>24457.5</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6" s="7">
         <v>0.57771347584740762</v>
       </c>
       <c r="T6" t="s">
@@ -14984,19 +14903,19 @@
         <v>0.108893350655486</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>936.57</v>
       </c>
-      <c r="C7" s="3" t="str">
+      <c r="C7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>CEN</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
-        <v>CEN</v>
-      </c>
-      <c r="D7">
-        <f>B7/1000</f>
         <v>0.93657000000000001</v>
       </c>
       <c r="F7" t="s">
@@ -15011,43 +14930,43 @@
       <c r="K7">
         <v>1.036</v>
       </c>
-      <c r="L7" s="8">
-        <f t="shared" si="1"/>
+      <c r="L7" s="7">
+        <f t="shared" si="2"/>
         <v>0.10461930589735793</v>
       </c>
       <c r="N7" t="s">
         <v>251</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="9">
         <v>6822.86</v>
       </c>
-      <c r="P7" s="9">
-        <f t="shared" si="2"/>
+      <c r="P7" s="8">
+        <f t="shared" si="3"/>
         <v>0.17174970296232153</v>
       </c>
       <c r="Q7">
         <v>3087</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R7" s="7">
         <v>7.2918389039801579E-2</v>
       </c>
       <c r="T7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>330</v>
       </c>
-      <c r="C8" s="3" t="str">
+      <c r="C8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>HBY</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>HBY</v>
-      </c>
-      <c r="D8">
-        <f>B8/1000</f>
         <v>0.33</v>
       </c>
       <c r="F8" t="s">
@@ -15062,43 +14981,43 @@
       <c r="K8">
         <v>0.8286</v>
       </c>
-      <c r="L8" s="8">
-        <f t="shared" si="1"/>
+      <c r="L8" s="7">
+        <f t="shared" si="2"/>
         <v>8.3675247940686079E-2</v>
       </c>
       <c r="N8" t="s">
         <v>255</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9">
         <v>6675.12</v>
       </c>
-      <c r="P8" s="9">
-        <f t="shared" si="2"/>
+      <c r="P8" s="8">
+        <f t="shared" si="3"/>
         <v>0.16803069053708442</v>
       </c>
       <c r="Q8">
         <v>4610</v>
       </c>
-      <c r="R8" s="8">
+      <c r="R8" s="7">
         <v>0.108893350655486</v>
       </c>
       <c r="T8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>52.309999999999995</v>
       </c>
-      <c r="C9" s="3" t="str">
+      <c r="C9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>NEL</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>NEL</v>
-      </c>
-      <c r="D9">
-        <f>B9/1000</f>
         <v>5.2309999999999995E-2</v>
       </c>
       <c r="F9" t="s">
@@ -15113,43 +15032,43 @@
       <c r="K9">
         <v>0.76200000000000001</v>
       </c>
-      <c r="L9" s="8">
-        <f t="shared" si="1"/>
+      <c r="L9" s="7">
+        <f t="shared" si="2"/>
         <v>7.6949721132998791E-2</v>
       </c>
       <c r="N9" t="s">
         <v>263</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="9">
         <v>4704.12</v>
       </c>
-      <c r="P9" s="9">
-        <f t="shared" si="2"/>
+      <c r="P9" s="8">
+        <f t="shared" si="3"/>
         <v>0.11841532915802405</v>
       </c>
       <c r="Q9">
         <v>1369</v>
       </c>
-      <c r="R9" s="8">
+      <c r="R9" s="7">
         <v>3.2337309554741941E-2</v>
       </c>
       <c r="T9" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>58.3</v>
       </c>
-      <c r="C10" s="3" t="str">
+      <c r="C10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>NIS</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
-        <v>NIS</v>
-      </c>
-      <c r="D10">
-        <f>B10/1000</f>
         <v>5.8299999999999998E-2</v>
       </c>
       <c r="F10" t="s">
@@ -15164,38 +15083,38 @@
       <c r="K10">
         <v>0.53700000000000003</v>
       </c>
-      <c r="L10" s="8">
-        <f t="shared" si="1"/>
+      <c r="L10" s="7">
+        <f t="shared" si="2"/>
         <v>5.4228346782703871E-2</v>
       </c>
       <c r="N10" t="s">
         <v>790</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="10">
         <v>3213.66</v>
       </c>
-      <c r="P10" s="9">
-        <f t="shared" si="2"/>
+      <c r="P10" s="8">
+        <f t="shared" si="3"/>
         <v>8.0896449644561691E-2</v>
       </c>
-      <c r="R10" s="8"/>
+      <c r="R10" s="7"/>
       <c r="T10" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>1907.3500000000001</v>
       </c>
-      <c r="C11" s="3" t="str">
+      <c r="C11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OTG</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="0"/>
-        <v>OTG</v>
-      </c>
-      <c r="D11">
-        <f>B11/1000</f>
         <v>1.9073500000000001</v>
       </c>
       <c r="F11" t="s">
@@ -15210,43 +15129,43 @@
       <c r="K11">
         <v>0.17299999999999999</v>
       </c>
-      <c r="L11" s="8">
-        <f t="shared" si="1"/>
+      <c r="L11" s="7">
+        <f t="shared" si="2"/>
         <v>1.7470212278226756E-2</v>
       </c>
       <c r="N11" t="s">
         <v>128</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9">
         <v>1483.86</v>
       </c>
-      <c r="P11" s="9">
-        <f t="shared" si="2"/>
+      <c r="P11" s="8">
+        <f t="shared" si="3"/>
         <v>3.7352739794993657E-2</v>
       </c>
       <c r="Q11">
         <v>9</v>
       </c>
-      <c r="R11" s="8">
+      <c r="R11" s="7">
         <v>2.1259005550962559E-4</v>
       </c>
       <c r="T11" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>1065.7</v>
       </c>
-      <c r="C12" s="3" t="str">
+      <c r="C12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>TRN</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="0"/>
-        <v>TRN</v>
-      </c>
-      <c r="D12">
-        <f>B12/1000</f>
         <v>1.0657000000000001</v>
       </c>
       <c r="F12" t="s">
@@ -15261,43 +15180,43 @@
       <c r="K12">
         <v>0.112</v>
       </c>
-      <c r="L12" s="8">
-        <f t="shared" si="1"/>
+      <c r="L12" s="7">
+        <f t="shared" si="2"/>
         <v>1.1310195232146804E-2</v>
       </c>
       <c r="N12" t="s">
         <v>120</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="9">
         <v>981.12</v>
       </c>
-      <c r="P12" s="9">
-        <f t="shared" si="2"/>
+      <c r="P12" s="8">
+        <f t="shared" si="3"/>
         <v>2.4697424330910045E-2</v>
       </c>
       <c r="Q12">
         <v>550</v>
       </c>
-      <c r="R12" s="8">
+      <c r="R12" s="7">
         <v>1.2991614503366009E-2</v>
       </c>
       <c r="T12" t="s">
         <v>810</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>237.7</v>
       </c>
-      <c r="C13" s="3" t="str">
+      <c r="C13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>WEL</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="0"/>
-        <v>WEL</v>
-      </c>
-      <c r="D13">
-        <f>B13/1000</f>
         <v>0.23769999999999999</v>
       </c>
       <c r="F13" t="s">
@@ -15312,24 +15231,24 @@
       <c r="K13">
         <v>5.6099999999999997E-2</v>
       </c>
-      <c r="L13" s="8">
-        <f t="shared" si="1"/>
+      <c r="L13" s="7">
+        <f t="shared" si="2"/>
         <v>5.6651960046735323E-3</v>
       </c>
       <c r="N13" t="s">
         <v>49</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="9">
         <v>460.29300000000001</v>
       </c>
-      <c r="P13" s="9">
-        <f t="shared" si="2"/>
+      <c r="P13" s="8">
+        <f t="shared" si="3"/>
         <v>1.1586810520168356E-2</v>
       </c>
       <c r="Q13">
         <v>417.5</v>
       </c>
-      <c r="R13" s="8">
+      <c r="R13" s="7">
         <v>9.8618164639187426E-3</v>
       </c>
       <c r="T13" t="s">
@@ -15339,19 +15258,19 @@
         <v>42335</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>3192.6</v>
       </c>
-      <c r="C14" s="3" t="str">
+      <c r="C14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>WTO</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="0"/>
-        <v>WTO</v>
-      </c>
-      <c r="D14">
-        <f>B14/1000</f>
         <v>3.1926000000000001</v>
       </c>
       <c r="F14" t="s">
@@ -15370,18 +15289,18 @@
       <c r="N14" t="s">
         <v>798</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="9">
         <v>-53.515000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>10179.01</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="3"/>
       <c r="F15" t="s">
         <v>789</v>
       </c>
@@ -15391,11 +15310,11 @@
       <c r="N15" t="s">
         <v>801</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="9">
         <v>-1152.3</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>120</v>
       </c>
@@ -15405,11 +15324,11 @@
       <c r="N16" t="s">
         <v>782</v>
       </c>
-      <c r="O16" s="10">
+      <c r="O16" s="9">
         <v>-39725.599999999999</v>
       </c>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>790</v>
       </c>
@@ -15417,8 +15336,8 @@
         <v>2.9215399999999998E-3</v>
       </c>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="H18" s="5">
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="4">
         <v>6.6791499999999999E-5</v>
       </c>
     </row>
@@ -15428,44 +15347,44 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4:R20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="K2" s="6" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K2" s="5" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="6" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>778</v>
       </c>
       <c r="B4" t="s">
@@ -15517,27 +15436,23 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>15.5</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>112</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1">
+      <c r="G5">
         <v>3.6</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1">
+      <c r="I5">
         <v>3.4000000000000004</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5">
         <v>134.5</v>
       </c>
       <c r="K5" t="s">
@@ -15572,31 +15487,29 @@
         <v>gt_cap.loc[idx["AKL", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>37</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>175</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6">
         <v>37.299999999999997</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6">
         <v>246.95</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6">
         <v>506.25</v>
       </c>
       <c r="K6" t="s">
@@ -15631,25 +15544,20 @@
         <v>gt_cap.loc[idx["BOP", [2020], "OCGT"], "unitsUpperLimit"] = 0.01 # GW_el</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>3.4000000000000004</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>4.6999999999999993</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1">
+      <c r="I7">
         <v>1749.6299999999997</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7">
         <v>1757.7299999999996</v>
       </c>
       <c r="L7" t="str">
@@ -15681,21 +15589,14 @@
         <v>gt_cap.loc[idx["CAN", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1">
+      <c r="I8">
         <v>936.57</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8">
         <v>936.57</v>
       </c>
       <c r="L8" t="str">
@@ -15727,25 +15628,20 @@
         <v>gt_cap.loc[idx["CEN", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>12.8</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>155</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1">
+      <c r="I9">
         <v>162.20000000000002</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9">
         <v>330</v>
       </c>
       <c r="L9" t="str">
@@ -15777,23 +15673,17 @@
         <v>gt_cap.loc[idx["HBY", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>0.60000000000000009</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1">
+      <c r="I10">
         <v>51.709999999999994</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10">
         <v>52.309999999999995</v>
       </c>
       <c r="L10" t="str">
@@ -15825,27 +15715,23 @@
         <v>gt_cap.loc[idx["NEL", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>18</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>25</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1">
+      <c r="I11">
         <v>5.5</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11">
         <v>58.3</v>
       </c>
       <c r="L11" t="str">
@@ -15877,23 +15763,17 @@
         <v>gt_cap.loc[idx["NIS", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>1.4</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1">
+      <c r="I12">
         <v>1905.95</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12">
         <v>1907.3500000000001</v>
       </c>
       <c r="L12" t="str">
@@ -15925,27 +15805,23 @@
         <v>gt_cap.loc[idx["OTG", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>377</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1">
+      <c r="G13">
         <v>78.599999999999994</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13">
         <v>435</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13">
         <v>175.10000000000002</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13">
         <v>1065.7</v>
       </c>
       <c r="L13" t="str">
@@ -15977,25 +15853,20 @@
         <v>gt_cap.loc[idx["TRN", [2020], "OCGT"], "unitsUpperLimit"] = 0.435 # GW_el</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>3.8000000000000003</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1">
+      <c r="G14">
         <v>10</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1">
+      <c r="I14">
         <v>223.89999999999998</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14">
         <v>237.7</v>
       </c>
       <c r="L14" t="str">
@@ -16027,31 +15898,29 @@
         <v>gt_cap.loc[idx["WEL", [2020], "OCGT"], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>45.9</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>385</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>836</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15">
         <v>750</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15">
         <v>92</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15">
         <v>1083.7</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15">
         <v>3192.6000000000004</v>
       </c>
       <c r="L15" t="str">
@@ -16083,45 +15952,45 @@
         <v>gt_cap.loc[idx["WTO", [2020], "OCGT"], "unitsUpperLimit"] = 0.092 # GW_el</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>129.6</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>762</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>112</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
         <v>178.29999999999998</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
         <v>1036</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16">
         <v>879.5</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16">
         <v>537</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16">
         <v>6544.61</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16">
         <v>10179.01</v>
       </c>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L17" t="str">
         <f>CONCATENATE($K$5, ".loc[idx[","""",A17,"""",", [2020], ", """",L16,"""",, "], ", """", "unitsUpperLimit", """", "] = ",IF(B17&gt;0,_xlfn.CONCAT(B17, " # GW_el"),"0"))</f>
         <v>gt_cap.loc[idx["", [2020], ""], "unitsUpperLimit"] = 0</v>
       </c>
     </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L19" t="str">
         <f>L6</f>
         <v>gt_cap.loc[idx["BOP", [2020], "BIO"], "unitsUpperLimit"] = 0.037 # GW_el</v>
@@ -16133,48 +16002,48 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3:N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>805</v>
       </c>
       <c r="B1" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>791</v>
       </c>
       <c r="M3" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>778</v>
       </c>
       <c r="B4">
@@ -16213,31 +16082,25 @@
       <c r="M4">
         <v>417.5</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="7">
         <f>M4/$M$12</f>
         <v>9.8618164639187426E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>38.1</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>550</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1">
+      <c r="H5">
         <v>7</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1">
+      <c r="K5">
         <v>595.1</v>
       </c>
       <c r="L5" t="s">
@@ -16246,31 +16109,25 @@
       <c r="M5">
         <v>4610</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="7">
         <f t="shared" ref="N5:N11" si="0">M5/$M$12</f>
         <v>0.108893350655486</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1">
+      <c r="G6">
         <v>1115</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1">
+      <c r="I6">
         <v>954</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6">
         <v>54</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6">
         <v>2123</v>
       </c>
       <c r="L6" t="s">
@@ -16279,31 +16136,25 @@
       <c r="M6">
         <v>550</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <f t="shared" si="0"/>
         <v>1.2991614503366009E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>1.2000000000000002</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1">
+      <c r="I7">
         <v>7961</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1">
+      <c r="K7">
         <v>7964.2</v>
       </c>
       <c r="L7" t="s">
@@ -16312,29 +16163,22 @@
       <c r="M7">
         <v>9</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <f t="shared" si="0"/>
         <v>2.1259005550962559E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>1068</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1">
+      <c r="I8">
         <v>1479</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1">
+      <c r="K8">
         <v>2547</v>
       </c>
       <c r="L8" t="s">
@@ -16343,31 +16187,25 @@
       <c r="M8">
         <v>7835</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="7">
         <f t="shared" si="0"/>
         <v>0.1850714538797685</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>48</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>9</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1">
+      <c r="I9">
         <v>467</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1">
+      <c r="K9">
         <v>524</v>
       </c>
       <c r="L9" t="s">
@@ -16376,29 +16214,22 @@
       <c r="M9">
         <v>3087</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <f t="shared" si="0"/>
         <v>7.2918389039801579E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>12.2</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1">
+      <c r="I10">
         <v>190</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1">
+      <c r="K10">
         <v>202.2</v>
       </c>
       <c r="L10" t="s">
@@ -16407,31 +16238,25 @@
       <c r="M10">
         <v>1369</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="7">
         <f t="shared" si="0"/>
         <v>3.2337309554741941E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>22</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11">
         <v>200</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1">
+      <c r="K11">
         <v>222</v>
       </c>
       <c r="L11" t="s">
@@ -16441,31 +16266,25 @@
         <f>GETPIVOTDATA("Avg_Ann_Gen_GWh",$A$3,"new_tech","Hydro")</f>
         <v>24457.5</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="7">
         <f t="shared" si="0"/>
         <v>0.57771347584740762</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>371</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>1.9</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1">
+      <c r="I12">
         <v>9602.5</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1">
+      <c r="K12">
         <v>9975.4</v>
       </c>
       <c r="L12" t="s">
@@ -16476,119 +16295,105 @@
         <v>42335</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>2200</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1">
+      <c r="H13">
         <v>230</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13">
         <v>118</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13">
         <v>780</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13">
         <v>3328</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>807.8</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>13</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1">
+      <c r="K14">
         <v>820.8</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>225</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>292.5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>2410</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1">
+      <c r="G15">
         <v>5541</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15">
         <v>2850</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15">
         <v>3686</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15">
         <v>535</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15">
         <v>15539.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>2485.1999999999998</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>417.5</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>4610</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
         <v>550</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
         <v>9</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16">
         <v>6856</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16">
         <v>3087</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16">
         <v>24457.5</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16">
         <v>1369</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16">
         <v>43841.2</v>
       </c>
     </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>7835</v>
       </c>
@@ -16602,44 +16407,44 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AL229"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL3" sqref="AL3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" customWidth="1"/>
-    <col min="5" max="6" width="16.08984375" customWidth="1"/>
-    <col min="7" max="7" width="14.08984375" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
-    <col min="9" max="9" width="17.7265625" customWidth="1"/>
-    <col min="10" max="10" width="18.1796875" customWidth="1"/>
-    <col min="11" max="11" width="24.90625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="11.36328125" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" customWidth="1"/>
-    <col min="16" max="16" width="15.54296875" customWidth="1"/>
-    <col min="17" max="17" width="13.81640625" customWidth="1"/>
-    <col min="18" max="18" width="13.7265625" customWidth="1"/>
-    <col min="19" max="20" width="10.453125" customWidth="1"/>
-    <col min="21" max="21" width="10.54296875" customWidth="1"/>
-    <col min="22" max="22" width="17.08984375" customWidth="1"/>
-    <col min="23" max="23" width="19.7265625" customWidth="1"/>
-    <col min="24" max="24" width="23.36328125" customWidth="1"/>
-    <col min="26" max="26" width="14.81640625" customWidth="1"/>
-    <col min="27" max="27" width="14.1796875" customWidth="1"/>
-    <col min="28" max="28" width="13.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" customWidth="1"/>
+    <col min="19" max="20" width="10.42578125" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" customWidth="1"/>
+    <col min="22" max="22" width="17.140625" customWidth="1"/>
+    <col min="23" max="23" width="19.7109375" customWidth="1"/>
+    <col min="24" max="24" width="23.42578125" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" customWidth="1"/>
+    <col min="27" max="27" width="14.140625" customWidth="1"/>
+    <col min="28" max="28" width="13.5703125" customWidth="1"/>
     <col min="29" max="29" width="13" customWidth="1"/>
-    <col min="30" max="30" width="15.08984375" customWidth="1"/>
-    <col min="31" max="31" width="9.54296875" customWidth="1"/>
-    <col min="32" max="32" width="15.26953125" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" customWidth="1"/>
+    <col min="31" max="31" width="9.5703125" customWidth="1"/>
+    <col min="32" max="32" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16755,7 +16560,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -16825,7 +16630,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -16895,7 +16700,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -16968,7 +16773,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -17041,7 +16846,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -17111,7 +16916,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -17181,7 +16986,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -17254,7 +17059,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -17327,7 +17132,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>92</v>
       </c>
@@ -17394,7 +17199,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -17467,7 +17272,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -17537,7 +17342,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -17607,7 +17412,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -17689,7 +17494,7 @@
         <v>COAL</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -17768,7 +17573,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -17841,7 +17646,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>133</v>
       </c>
@@ -17905,7 +17710,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -17972,7 +17777,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -18039,7 +17844,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>143</v>
       </c>
@@ -18106,7 +17911,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>146</v>
       </c>
@@ -18173,7 +17978,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>147</v>
       </c>
@@ -18240,7 +18045,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>152</v>
       </c>
@@ -18307,7 +18112,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>154</v>
       </c>
@@ -18374,7 +18179,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>155</v>
       </c>
@@ -18441,7 +18246,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>156</v>
       </c>
@@ -18508,7 +18313,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>160</v>
       </c>
@@ -18575,7 +18380,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>164</v>
       </c>
@@ -18642,7 +18447,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>166</v>
       </c>
@@ -18709,7 +18514,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>165</v>
       </c>
@@ -18776,7 +18581,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>167</v>
       </c>
@@ -18843,7 +18648,7 @@
         <v>DIE</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -18925,7 +18730,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>191</v>
       </c>
@@ -19007,7 +18812,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>207</v>
       </c>
@@ -19092,7 +18897,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>214</v>
       </c>
@@ -19177,7 +18982,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>220</v>
       </c>
@@ -19262,7 +19067,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>234</v>
       </c>
@@ -19344,7 +19149,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>195</v>
       </c>
@@ -19429,7 +19234,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>187</v>
       </c>
@@ -19514,7 +19319,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>199</v>
       </c>
@@ -19599,7 +19404,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>204</v>
       </c>
@@ -19684,7 +19489,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>208</v>
       </c>
@@ -19769,7 +19574,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>215</v>
       </c>
@@ -19857,7 +19662,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>223</v>
       </c>
@@ -19942,7 +19747,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>227</v>
       </c>
@@ -20027,7 +19832,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>233</v>
       </c>
@@ -20112,7 +19917,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>237</v>
       </c>
@@ -20203,7 +20008,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -20291,7 +20096,7 @@
         <v>geoth</v>
       </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>245</v>
       </c>
@@ -20379,7 +20184,7 @@
         <v>GT</v>
       </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>252</v>
       </c>
@@ -20455,7 +20260,7 @@
         <v>CCGT</v>
       </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>256</v>
       </c>
@@ -20537,7 +20342,7 @@
         <v>CCGT</v>
       </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>262</v>
       </c>
@@ -20613,7 +20418,7 @@
         <v>OCGT</v>
       </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>264</v>
       </c>
@@ -20686,7 +20491,7 @@
         <v>OCGT</v>
       </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>269</v>
       </c>
@@ -20771,7 +20576,7 @@
         <v>OCGT</v>
       </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>273</v>
       </c>
@@ -20859,7 +20664,7 @@
         <v>GT</v>
       </c>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>279</v>
       </c>
@@ -20938,7 +20743,7 @@
         <v>OCGT</v>
       </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>280</v>
       </c>
@@ -21017,7 +20822,7 @@
         <v>OCGT</v>
       </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>283</v>
       </c>
@@ -21090,7 +20895,7 @@
         <v>GT</v>
       </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>285</v>
       </c>
@@ -21163,7 +20968,7 @@
         <v>OCGT</v>
       </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>289</v>
       </c>
@@ -21242,7 +21047,7 @@
         <v>OCGT</v>
       </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>293</v>
       </c>
@@ -21315,7 +21120,7 @@
         <v>GT</v>
       </c>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>296</v>
       </c>
@@ -21394,7 +21199,7 @@
         <v>GT</v>
       </c>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>298</v>
       </c>
@@ -21470,7 +21275,7 @@
         <v>GT</v>
       </c>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>303</v>
       </c>
@@ -21537,7 +21342,7 @@
         <v>GT</v>
       </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>306</v>
       </c>
@@ -21601,7 +21406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>310</v>
       </c>
@@ -21665,7 +21470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>314</v>
       </c>
@@ -21729,7 +21534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>317</v>
       </c>
@@ -21793,7 +21598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>321</v>
       </c>
@@ -21857,7 +21662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>327</v>
       </c>
@@ -21921,7 +21726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>330</v>
       </c>
@@ -21985,7 +21790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>333</v>
       </c>
@@ -22049,7 +21854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>334</v>
       </c>
@@ -22113,7 +21918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>337</v>
       </c>
@@ -22177,7 +21982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>342</v>
       </c>
@@ -22241,7 +22046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>344</v>
       </c>
@@ -22305,7 +22110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>346</v>
       </c>
@@ -22369,7 +22174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>348</v>
       </c>
@@ -22433,7 +22238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>352</v>
       </c>
@@ -22497,7 +22302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>353</v>
       </c>
@@ -22561,7 +22366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>357</v>
       </c>
@@ -22625,7 +22430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>359</v>
       </c>
@@ -22689,7 +22494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>361</v>
       </c>
@@ -22753,7 +22558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>363</v>
       </c>
@@ -22817,7 +22622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>367</v>
       </c>
@@ -22881,7 +22686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>369</v>
       </c>
@@ -22945,7 +22750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>372</v>
       </c>
@@ -23009,7 +22814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>377</v>
       </c>
@@ -23073,7 +22878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>379</v>
       </c>
@@ -23137,7 +22942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>382</v>
       </c>
@@ -23201,7 +23006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>386</v>
       </c>
@@ -23265,7 +23070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>389</v>
       </c>
@@ -23329,7 +23134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>393</v>
       </c>
@@ -23393,7 +23198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>396</v>
       </c>
@@ -23457,7 +23262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>397</v>
       </c>
@@ -23521,7 +23326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>399</v>
       </c>
@@ -23585,7 +23390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>402</v>
       </c>
@@ -23652,7 +23457,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>406</v>
       </c>
@@ -23740,7 +23545,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>415</v>
       </c>
@@ -23840,7 +23645,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>423</v>
       </c>
@@ -23937,7 +23742,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>430</v>
       </c>
@@ -24034,7 +23839,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>434</v>
       </c>
@@ -24134,7 +23939,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>438</v>
       </c>
@@ -24234,7 +24039,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>445</v>
       </c>
@@ -24334,7 +24139,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>449</v>
       </c>
@@ -24434,7 +24239,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>453</v>
       </c>
@@ -24534,7 +24339,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>456</v>
       </c>
@@ -24634,7 +24439,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>461</v>
       </c>
@@ -24734,7 +24539,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>464</v>
       </c>
@@ -24834,7 +24639,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>465</v>
       </c>
@@ -24934,7 +24739,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>469</v>
       </c>
@@ -25031,7 +24836,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>470</v>
       </c>
@@ -25128,7 +24933,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="113" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>474</v>
       </c>
@@ -25225,7 +25030,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="114" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>418</v>
       </c>
@@ -25325,7 +25130,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="115" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>478</v>
       </c>
@@ -25425,7 +25230,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="116" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>482</v>
       </c>
@@ -25513,7 +25318,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="117" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>487</v>
       </c>
@@ -25610,7 +25415,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="118" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>489</v>
       </c>
@@ -25707,7 +25512,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="119" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>491</v>
       </c>
@@ -25807,7 +25612,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="120" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>498</v>
       </c>
@@ -25901,7 +25706,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="121" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>504</v>
       </c>
@@ -26001,7 +25806,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="122" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>507</v>
       </c>
@@ -26092,7 +25897,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="123" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>511</v>
       </c>
@@ -26192,7 +25997,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="124" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>513</v>
       </c>
@@ -26280,7 +26085,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="125" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>519</v>
       </c>
@@ -26380,7 +26185,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="126" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>521</v>
       </c>
@@ -26474,7 +26279,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="127" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>527</v>
       </c>
@@ -26562,7 +26367,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="128" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>530</v>
       </c>
@@ -26662,7 +26467,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="129" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>534</v>
       </c>
@@ -26753,7 +26558,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="130" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>536</v>
       </c>
@@ -26847,7 +26652,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="131" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>540</v>
       </c>
@@ -26935,7 +26740,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="132" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>541</v>
       </c>
@@ -27029,7 +26834,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="133" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>546</v>
       </c>
@@ -27123,7 +26928,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="134" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>547</v>
       </c>
@@ -27208,7 +27013,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="135" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>552</v>
       </c>
@@ -27302,7 +27107,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="136" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>555</v>
       </c>
@@ -27396,7 +27201,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="137" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>560</v>
       </c>
@@ -27490,7 +27295,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="138" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>561</v>
       </c>
@@ -27584,7 +27389,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="139" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>562</v>
       </c>
@@ -27654,7 +27459,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="140" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>566</v>
       </c>
@@ -27745,7 +27550,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="141" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>572</v>
       </c>
@@ -27815,7 +27620,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="142" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>575</v>
       </c>
@@ -27897,7 +27702,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="143" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>577</v>
       </c>
@@ -27973,7 +27778,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="144" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>580</v>
       </c>
@@ -28043,7 +27848,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="145" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>583</v>
       </c>
@@ -28137,7 +27942,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="146" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>584</v>
       </c>
@@ -28225,7 +28030,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="147" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>585</v>
       </c>
@@ -28295,7 +28100,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="148" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>587</v>
       </c>
@@ -28365,7 +28170,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="149" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>588</v>
       </c>
@@ -28435,7 +28240,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="150" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>590</v>
       </c>
@@ -28505,7 +28310,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="151" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>591</v>
       </c>
@@ -28575,7 +28380,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="152" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>594</v>
       </c>
@@ -28657,7 +28462,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="153" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>595</v>
       </c>
@@ -28727,7 +28532,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="154" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>598</v>
       </c>
@@ -28797,7 +28602,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="155" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>600</v>
       </c>
@@ -28888,7 +28693,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="156" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>602</v>
       </c>
@@ -28970,7 +28775,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="157" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>603</v>
       </c>
@@ -29046,7 +28851,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="158" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>606</v>
       </c>
@@ -29116,7 +28921,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="159" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>609</v>
       </c>
@@ -29201,7 +29006,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="160" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>612</v>
       </c>
@@ -29274,7 +29079,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="161" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>614</v>
       </c>
@@ -29344,7 +29149,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="162" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>615</v>
       </c>
@@ -29414,7 +29219,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="163" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>616</v>
       </c>
@@ -29499,7 +29304,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="164" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>617</v>
       </c>
@@ -29593,7 +29398,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="165" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>618</v>
       </c>
@@ -29663,7 +29468,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="166" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>620</v>
       </c>
@@ -29748,7 +29553,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="167" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>621</v>
       </c>
@@ -29818,7 +29623,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="168" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>624</v>
       </c>
@@ -29900,7 +29705,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="169" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>625</v>
       </c>
@@ -29970,7 +29775,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="170" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>626</v>
       </c>
@@ -30040,7 +29845,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="171" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>629</v>
       </c>
@@ -30134,7 +29939,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="172" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>631</v>
       </c>
@@ -30204,7 +30009,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="173" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>632</v>
       </c>
@@ -30277,7 +30082,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="174" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>633</v>
       </c>
@@ -30362,7 +30167,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="175" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>634</v>
       </c>
@@ -30432,7 +30237,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="176" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>637</v>
       </c>
@@ -30502,7 +30307,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="177" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>638</v>
       </c>
@@ -30587,7 +30392,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="178" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>641</v>
       </c>
@@ -30654,7 +30459,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="179" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>645</v>
       </c>
@@ -30724,7 +30529,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="180" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>648</v>
       </c>
@@ -30803,7 +30608,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="181" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>650</v>
       </c>
@@ -30870,7 +30675,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="182" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>654</v>
       </c>
@@ -30937,7 +30742,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="183" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>656</v>
       </c>
@@ -31019,7 +30824,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="184" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>658</v>
       </c>
@@ -31104,7 +30909,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="185" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>659</v>
       </c>
@@ -31174,7 +30979,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="186" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>662</v>
       </c>
@@ -31268,7 +31073,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="187" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>663</v>
       </c>
@@ -31335,7 +31140,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="188" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>666</v>
       </c>
@@ -31402,7 +31207,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="189" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>668</v>
       </c>
@@ -31469,7 +31274,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="190" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>671</v>
       </c>
@@ -31548,7 +31353,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="191" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>675</v>
       </c>
@@ -31615,7 +31420,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="192" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>676</v>
       </c>
@@ -31682,7 +31487,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="193" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>678</v>
       </c>
@@ -31752,7 +31557,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="194" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>682</v>
       </c>
@@ -31819,7 +31624,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="195" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>683</v>
       </c>
@@ -31886,7 +31691,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="196" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>685</v>
       </c>
@@ -31953,7 +31758,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="197" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>687</v>
       </c>
@@ -32020,7 +31825,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="198" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>688</v>
       </c>
@@ -32087,7 +31892,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="199" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>691</v>
       </c>
@@ -32154,7 +31959,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="200" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>692</v>
       </c>
@@ -32221,7 +32026,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="201" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>693</v>
       </c>
@@ -32288,7 +32093,7 @@
         <v>Hydro</v>
       </c>
     </row>
-    <row r="202" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>695</v>
       </c>
@@ -32361,7 +32166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>700</v>
       </c>
@@ -32428,7 +32233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>703</v>
       </c>
@@ -32501,7 +32306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>707</v>
       </c>
@@ -32571,7 +32376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>711</v>
       </c>
@@ -32641,7 +32446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>715</v>
       </c>
@@ -32714,7 +32519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>720</v>
       </c>
@@ -32787,7 +32592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>722</v>
       </c>
@@ -32857,7 +32662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>724</v>
       </c>
@@ -32927,7 +32732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>728</v>
       </c>
@@ -32994,7 +32799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>730</v>
       </c>
@@ -33061,7 +32866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>732</v>
       </c>
@@ -33128,7 +32933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>734</v>
       </c>
@@ -33195,7 +33000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>738</v>
       </c>
@@ -33256,7 +33061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>739</v>
       </c>
@@ -33323,7 +33128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>741</v>
       </c>
@@ -33393,7 +33198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>743</v>
       </c>
@@ -33460,7 +33265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>746</v>
       </c>
@@ -33527,7 +33332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>748</v>
       </c>
@@ -33594,7 +33399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>750</v>
       </c>
@@ -33658,7 +33463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>753</v>
       </c>
@@ -33728,7 +33533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>760</v>
       </c>
@@ -33792,7 +33597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>761</v>
       </c>
@@ -33859,7 +33664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>763</v>
       </c>
@@ -33944,7 +33749,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="226" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>769</v>
       </c>
@@ -34011,7 +33816,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="227" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>772</v>
       </c>
@@ -34078,7 +33883,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="228" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>775</v>
       </c>
@@ -34145,7 +33950,7 @@
         <v>BIO</v>
       </c>
     </row>
-    <row r="229" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>776</v>
       </c>

</xml_diff>